<commit_message>
make export purchase order get parameter for status(s)
</commit_message>
<xml_diff>
--- a/report/purchaseOrders_template.xlsx
+++ b/report/purchaseOrders_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/i022021/dev/alonandella/dolibarr-extension/report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CEFE38C-9AF2-F14A-AD88-2CBAD6B37B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B712DE4D-C52E-E547-96F7-75BF437DF1B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>#</t>
   </si>
@@ -64,9 +64,6 @@
     <t>{ord:approver2}</t>
   </si>
   <si>
-    <t xml:space="preserve">הזמנות רכש מאושרות </t>
-  </si>
-  <si>
     <t>תאריך</t>
   </si>
   <si>
@@ -77,6 +74,15 @@
   </si>
   <si>
     <t>מס׳ הזמנה</t>
+  </si>
+  <si>
+    <t xml:space="preserve">הזמנות רכש </t>
+  </si>
+  <si>
+    <t>{header:title}</t>
+  </si>
+  <si>
+    <t>סטטוס:</t>
   </si>
 </sst>
 </file>
@@ -144,7 +150,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -195,11 +201,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="22"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -219,14 +234,23 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -535,7 +559,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScale="226" zoomScaleNormal="226" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -552,21 +576,25 @@
     <col min="10" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:9" s="12" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="8"/>
+      <c r="H1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="11" t="s">
         <v>15</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -574,7 +602,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>3</v>
@@ -600,7 +628,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>2</v>
@@ -624,7 +652,7 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A1:C1"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>